<commit_message>
Manipulation df to list done
</commit_message>
<xml_diff>
--- a/Neraca.xlsx
+++ b/Neraca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ngoding\KP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24968F7F-A527-4C0F-8914-BE015D002C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D540B3F-1BCD-4EEC-B503-AC46E5740EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="26">
   <si>
     <t>Kabupaten/Kota</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Tahun 2021</t>
-  </si>
-  <si>
-    <t>Persentase</t>
   </si>
 </sst>
 </file>
@@ -263,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,7 +291,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -305,20 +301,9 @@
     <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -333,6 +318,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +543,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <selection pane="topRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F6" sqref="F6"/>
+      <selection pane="topRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1674,9 @@
       <c r="E1" s="8">
         <v>2021</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -1709,23 +1699,26 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="23">
         <v>11.44</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="23">
         <v>11.45</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="23">
         <v>11.62</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="23">
         <v>11.63</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="29">
+        <f>AVERAGE(B2:E2)</f>
+        <v>11.535</v>
+      </c>
+      <c r="G2" s="28"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -1747,23 +1740,26 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="25">
         <v>11.31</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="25">
         <v>11.32</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="25">
         <v>11.33</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="25">
         <v>11.34</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="29">
+        <f t="shared" ref="F3:F21" si="0">AVERAGE(B3:E3)</f>
+        <v>11.324999999999999</v>
+      </c>
+      <c r="G3" s="28"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -1785,23 +1781,26 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="25">
         <v>11.33</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="25">
         <v>11.34</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="25">
         <v>11.58</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="25">
         <v>11.59</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="9"/>
+      <c r="F4" s="29">
+        <f t="shared" si="0"/>
+        <v>11.46</v>
+      </c>
+      <c r="G4" s="28"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -1823,23 +1822,26 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="23">
         <v>11.01</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="23">
         <v>11.02</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="23">
         <v>11.03</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="23">
         <v>11.04</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="29">
+        <f t="shared" si="0"/>
+        <v>11.025</v>
+      </c>
+      <c r="G5" s="28"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -1861,23 +1863,26 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="23">
         <v>10.46</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="23">
         <v>10.72</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="23">
         <v>10.73</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="23">
         <v>10.81</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="29">
+        <f t="shared" si="0"/>
+        <v>10.68</v>
+      </c>
+      <c r="G6" s="28"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -1899,23 +1904,26 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="25">
         <v>10.36</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="25">
         <v>10.37</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="25">
         <v>10.59</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="25">
         <v>10.67</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="29">
+        <f t="shared" si="0"/>
+        <v>10.497499999999999</v>
+      </c>
+      <c r="G7" s="28"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -1937,23 +1945,26 @@
       <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="25">
         <v>9.94</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="25">
         <v>9.9700000000000006</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="25">
         <v>10.17</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="25">
         <v>10.32</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="29">
+        <f t="shared" si="0"/>
+        <v>10.1</v>
+      </c>
+      <c r="G8" s="28"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -1975,23 +1986,26 @@
       <c r="Z8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="23">
         <v>8.76</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="23">
         <v>8.92</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="23">
         <v>8.99</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="23">
         <v>9.07</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="29">
+        <f t="shared" si="0"/>
+        <v>8.9350000000000005</v>
+      </c>
+      <c r="G9" s="28"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -2013,23 +2027,26 @@
       <c r="Z9" s="9"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="25">
         <v>8.69</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="25">
         <v>8.85</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="25">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="25">
         <v>8.9700000000000006</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="29">
+        <f t="shared" si="0"/>
+        <v>8.8674999999999997</v>
+      </c>
+      <c r="G10" s="28"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -2051,23 +2068,26 @@
       <c r="Z10" s="9"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="25">
         <v>8.44</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="25">
         <v>8.4499999999999993</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="25">
         <v>8.61</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="25">
         <v>8.6199999999999992</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="29">
+        <f t="shared" si="0"/>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="G11" s="28"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2089,23 +2109,26 @@
       <c r="Z11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="25">
         <v>8.25</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="25">
         <v>8.4600000000000009</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="25">
         <v>8.4700000000000006</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="25">
         <v>8.5500000000000007</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="29">
+        <f t="shared" si="0"/>
+        <v>8.432500000000001</v>
+      </c>
+      <c r="G12" s="28"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -2127,23 +2150,26 @@
       <c r="Z12" s="9"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="23">
         <v>7.86</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="23">
         <v>8.06</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="23">
         <v>8.19</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="23">
         <v>8.27</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="29">
+        <f t="shared" si="0"/>
+        <v>8.0949999999999989</v>
+      </c>
+      <c r="G13" s="28"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2165,23 +2191,26 @@
       <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="23">
         <v>8.14</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="23">
         <v>8.25</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="23">
         <v>8.26</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="23">
         <v>8.27</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="29">
+        <f t="shared" si="0"/>
+        <v>8.23</v>
+      </c>
+      <c r="G14" s="28"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -2203,23 +2232,26 @@
       <c r="Z14" s="9"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="23">
         <v>8.15</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="23">
         <v>8.16</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="23">
         <v>8.2799999999999994</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="23">
         <v>8.32</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="29">
+        <f t="shared" si="0"/>
+        <v>8.2275000000000009</v>
+      </c>
+      <c r="G15" s="28"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -2241,23 +2273,26 @@
       <c r="Z15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="23">
         <v>7.77</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="23">
         <v>8.1</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="23">
         <v>8.11</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="23">
         <v>8.1199999999999992</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="9"/>
+      <c r="F16" s="29">
+        <f t="shared" si="0"/>
+        <v>8.0249999999999986</v>
+      </c>
+      <c r="G16" s="28"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -2279,23 +2314,26 @@
       <c r="Z16" s="9"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="23">
         <v>7.5</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="23">
         <v>7.86</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="23">
         <v>7.87</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="23">
         <v>7.88</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="9"/>
+      <c r="F17" s="29">
+        <f t="shared" si="0"/>
+        <v>7.7774999999999999</v>
+      </c>
+      <c r="G17" s="28"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -2317,23 +2355,26 @@
       <c r="Z17" s="9"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="25">
         <v>7.66</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="25">
         <v>7.86</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="25">
         <v>8.09</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="25">
         <v>8.1</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="29">
+        <f t="shared" si="0"/>
+        <v>7.9275000000000002</v>
+      </c>
+      <c r="G18" s="28"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -2355,23 +2396,26 @@
       <c r="Z18" s="9"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="23">
         <v>7.97</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="23">
         <v>7.98</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="23">
         <v>7.99</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="23">
         <v>8.07</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="9"/>
+      <c r="F19" s="29">
+        <f t="shared" si="0"/>
+        <v>8.0024999999999995</v>
+      </c>
+      <c r="G19" s="28"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -2393,23 +2437,26 @@
       <c r="Z19" s="9"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="25">
         <v>7.84</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="25">
         <v>7.85</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="25">
         <v>7.86</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="25">
         <v>7.87</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="9"/>
+      <c r="F20" s="29">
+        <f t="shared" si="0"/>
+        <v>7.8550000000000004</v>
+      </c>
+      <c r="G20" s="28"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -2431,23 +2478,26 @@
       <c r="Z20" s="9"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="25">
         <v>6.95</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="25">
         <v>7.08</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="25">
         <v>7.09</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="25">
         <v>7.2</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="9"/>
+      <c r="F21" s="29">
+        <f t="shared" si="0"/>
+        <v>7.08</v>
+      </c>
+      <c r="G21" s="28"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -2686,7 +2736,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I12" sqref="I12"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2710,7 +2760,9 @@
       <c r="E1" s="8">
         <v>2021</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -2748,8 +2800,11 @@
       <c r="E2" s="14">
         <v>16.53</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="12">
+        <f>AVERAGE(B2:E2)</f>
+        <v>16.515000000000001</v>
+      </c>
+      <c r="G2" s="28"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2786,8 +2841,11 @@
       <c r="E3" s="11">
         <v>15.07</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F21" si="0">AVERAGE(B3:E3)</f>
+        <v>15.055</v>
+      </c>
+      <c r="G3" s="28"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2824,8 +2882,11 @@
       <c r="E4" s="14">
         <v>14.98</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="9"/>
+      <c r="F4" s="12">
+        <f t="shared" si="0"/>
+        <v>14.965</v>
+      </c>
+      <c r="G4" s="28"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2862,8 +2923,11 @@
       <c r="E5" s="14">
         <v>14.55</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>14.535</v>
+      </c>
+      <c r="G5" s="28"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2900,8 +2964,11 @@
       <c r="E6" s="14">
         <v>14.34</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>14.217500000000001</v>
+      </c>
+      <c r="G6" s="28"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2938,8 +3005,11 @@
       <c r="E7" s="11">
         <v>14.33</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="12">
+        <f t="shared" si="0"/>
+        <v>14.315</v>
+      </c>
+      <c r="G7" s="28"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2976,8 +3046,11 @@
       <c r="E8" s="11">
         <v>14.27</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="12">
+        <f t="shared" si="0"/>
+        <v>14.254999999999999</v>
+      </c>
+      <c r="G8" s="28"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -3014,8 +3087,11 @@
       <c r="E9" s="11">
         <v>14.09</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="12">
+        <f t="shared" si="0"/>
+        <v>14.017500000000002</v>
+      </c>
+      <c r="G9" s="28"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -3052,8 +3128,11 @@
       <c r="E10" s="14">
         <v>13.88</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>13.865</v>
+      </c>
+      <c r="G10" s="28"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -3090,8 +3169,11 @@
       <c r="E11" s="11">
         <v>13.68</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>13.635</v>
+      </c>
+      <c r="G11" s="28"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -3128,8 +3210,11 @@
       <c r="E12" s="11">
         <v>13.68</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>13.477500000000001</v>
+      </c>
+      <c r="G12" s="28"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -3166,8 +3251,11 @@
       <c r="E13" s="11">
         <v>13.33</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>13.315</v>
+      </c>
+      <c r="G13" s="28"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -3204,8 +3292,11 @@
       <c r="E14" s="11">
         <v>13.3</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>13.285</v>
+      </c>
+      <c r="G14" s="28"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3242,8 +3333,11 @@
       <c r="E15" s="14">
         <v>13.18</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>13.165000000000001</v>
+      </c>
+      <c r="G15" s="28"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -3280,8 +3374,11 @@
       <c r="E16" s="14">
         <v>13.05</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="9"/>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>13.035</v>
+      </c>
+      <c r="G16" s="28"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -3318,8 +3415,11 @@
       <c r="E17" s="14">
         <v>12.89</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="9"/>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>12.715</v>
+      </c>
+      <c r="G17" s="28"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -3356,8 +3456,11 @@
       <c r="E18" s="14">
         <v>12.81</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>12.795000000000002</v>
+      </c>
+      <c r="G18" s="28"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -3394,8 +3497,11 @@
       <c r="E19" s="11">
         <v>12.72</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="9"/>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>12.705</v>
+      </c>
+      <c r="G19" s="28"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -3432,8 +3538,11 @@
       <c r="E20" s="14">
         <v>12.44</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="9"/>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>12.424999999999999</v>
+      </c>
+      <c r="G20" s="28"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -3470,8 +3579,11 @@
       <c r="E21" s="11">
         <v>12.38</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="9"/>
+      <c r="F21" s="12">
+        <f t="shared" si="0"/>
+        <v>12.365</v>
+      </c>
+      <c r="G21" s="28"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -25064,7 +25176,7 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E21"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25088,7 +25200,9 @@
       <c r="E1" s="8">
         <v>2021</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -25114,19 +25228,22 @@
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>14312</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="19">
         <v>14728</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="19">
         <v>14481</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="19">
         <v>14540</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="18">
+        <f>AVERAGE(B2:E2)</f>
+        <v>14515.25</v>
+      </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -25152,19 +25269,22 @@
       <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>13035</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>13586</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <v>13282</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="19">
         <v>13331</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="18">
+        <f t="shared" ref="F3:F21" si="0">AVERAGE(B3:E3)</f>
+        <v>13308.5</v>
+      </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -25190,19 +25310,22 @@
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>13114</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>13464</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>13281</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>13317</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="18">
+        <f t="shared" si="0"/>
+        <v>13294</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -25228,19 +25351,22 @@
       <c r="A5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>12611</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>12958</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="19">
         <v>12796</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="19">
         <v>12818</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="18">
+        <f t="shared" si="0"/>
+        <v>12795.75</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -25266,19 +25392,22 @@
       <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>11968</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>12337</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>12117</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>12168</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="18">
+        <f t="shared" si="0"/>
+        <v>12147.5</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -25304,19 +25433,22 @@
       <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>11189</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>11431</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <v>11273</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="19">
         <v>11324</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="18">
+        <f t="shared" si="0"/>
+        <v>11304.25</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -25342,19 +25474,22 @@
       <c r="A8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>10919</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>11158</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>10998</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>11050</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="18">
+        <f t="shared" si="0"/>
+        <v>11031.25</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -25380,19 +25515,22 @@
       <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>10638</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>10925</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>10733</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>10790</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="18">
+        <f t="shared" si="0"/>
+        <v>10771.5</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -25418,19 +25556,22 @@
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>10440</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>11013</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>10734</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>10754</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="18">
+        <f t="shared" si="0"/>
+        <v>10735.25</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -25456,19 +25597,22 @@
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>10417</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>10709</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="19">
         <v>10588</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <v>10616</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="18">
+        <f t="shared" si="0"/>
+        <v>10582.5</v>
+      </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -25494,19 +25638,22 @@
       <c r="A12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>10277</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>10395</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>10361</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>10389</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="18">
+        <f t="shared" si="0"/>
+        <v>10355.5</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -25532,19 +25679,22 @@
       <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>10199</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>10505</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>10325</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>10367</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="18">
+        <f t="shared" si="0"/>
+        <v>10349</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -25570,19 +25720,22 @@
       <c r="A14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="19">
         <v>10035</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="19">
         <v>10309</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="19">
         <v>10171</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="19">
         <v>10215</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="18">
+        <f t="shared" si="0"/>
+        <v>10182.5</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -25608,19 +25761,22 @@
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="19">
         <v>9765</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>10238</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>10182</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <v>10195</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="18">
+        <f t="shared" si="0"/>
+        <v>10095</v>
+      </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -25646,19 +25802,22 @@
       <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="17">
         <v>9500</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="17">
         <v>9842</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>9596</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <v>9668</v>
       </c>
-      <c r="F16" s="24"/>
+      <c r="F16" s="18">
+        <f t="shared" si="0"/>
+        <v>9651.5</v>
+      </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -25684,19 +25843,22 @@
       <c r="A17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>9489</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>9780</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <v>9651</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <v>9662</v>
       </c>
-      <c r="F17" s="23"/>
+      <c r="F17" s="18">
+        <f t="shared" si="0"/>
+        <v>9645.5</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -25722,19 +25884,22 @@
       <c r="A18" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="17">
         <v>9089</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>9444</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <v>9212</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="17">
         <v>9270</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="18">
+        <f t="shared" si="0"/>
+        <v>9253.75</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -25760,19 +25925,22 @@
       <c r="A19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="17">
         <v>8979</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <v>9180</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <v>9047</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="17">
         <v>9089</v>
       </c>
-      <c r="F19" s="23"/>
+      <c r="F19" s="18">
+        <f t="shared" si="0"/>
+        <v>9073.75</v>
+      </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -25798,19 +25966,22 @@
       <c r="A20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="19">
         <v>8238</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="19">
         <v>8599</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="19">
         <v>8425</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="19">
         <v>8440</v>
       </c>
-      <c r="F20" s="24"/>
+      <c r="F20" s="18">
+        <f t="shared" si="0"/>
+        <v>8425.5</v>
+      </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -25836,19 +26007,22 @@
       <c r="A21" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="19">
         <v>6211</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <v>6429</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
         <v>6281</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="19">
         <v>6321</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="F21" s="18">
+        <f t="shared" si="0"/>
+        <v>6310.5</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -25991,9 +26165,9 @@
   </sheetPr>
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H21" sqref="H21"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26002,7 +26176,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -26017,12 +26191,10 @@
       <c r="E1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -26044,29 +26216,26 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="21">
         <v>82.25</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="21">
         <v>82.68</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="21">
         <v>82.82</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="21">
         <v>82.9</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="16">
         <f>AVERAGE(B2:E2)</f>
         <v>82.662499999999994</v>
       </c>
-      <c r="G2" s="34">
-        <f>E2-D2</f>
-        <v>8.0000000000012506E-2</v>
-      </c>
+      <c r="G2" s="28"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -26088,29 +26257,26 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="21">
         <v>80.11</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="21">
         <v>80.709999999999994</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="21">
         <v>80.58</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="21">
         <v>80.7</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <f t="shared" ref="F3:F21" si="0">AVERAGE(B3:E3)</f>
         <v>80.524999999999991</v>
       </c>
-      <c r="G3" s="34">
-        <f t="shared" ref="G3:G21" si="1">E3-D3</f>
-        <v>0.12000000000000455</v>
-      </c>
+      <c r="G3" s="28"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -26147,14 +26313,11 @@
       <c r="E4" s="11">
         <v>79.08</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <f t="shared" si="0"/>
         <v>78.790000000000006</v>
       </c>
-      <c r="G4" s="34">
-        <f t="shared" si="1"/>
-        <v>0.17999999999999261</v>
-      </c>
+      <c r="G4" s="28"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -26191,14 +26354,11 @@
       <c r="E5" s="11">
         <v>78.41</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <f t="shared" si="0"/>
         <v>78.242500000000007</v>
       </c>
-      <c r="G5" s="34">
-        <f t="shared" si="1"/>
-        <v>0.11999999999999034</v>
-      </c>
+      <c r="G5" s="28"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -26235,14 +26395,11 @@
       <c r="E6" s="11">
         <v>77.97</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <f t="shared" si="0"/>
         <v>77.800000000000011</v>
       </c>
-      <c r="G6" s="34">
-        <f t="shared" si="1"/>
-        <v>3.9999999999992042E-2</v>
-      </c>
+      <c r="G6" s="28"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -26264,29 +26421,26 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="21">
         <v>76.260000000000005</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="21">
         <v>76.7</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="21">
         <v>76.900000000000006</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="21">
         <v>77.069999999999993</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <f t="shared" si="0"/>
         <v>76.732500000000002</v>
       </c>
-      <c r="G7" s="34">
-        <f t="shared" si="1"/>
-        <v>0.16999999999998749</v>
-      </c>
+      <c r="G7" s="28"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -26308,29 +26462,26 @@
       <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="21">
         <v>71.72</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="21">
         <v>72.39</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="21">
         <v>72.64</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="21">
         <v>72.88</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
         <v>72.407499999999999</v>
       </c>
-      <c r="G8" s="34">
-        <f t="shared" si="1"/>
-        <v>0.23999999999999488</v>
-      </c>
+      <c r="G8" s="28"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -26367,14 +26518,11 @@
       <c r="E9" s="11">
         <v>72.650000000000006</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <f t="shared" si="0"/>
         <v>72.287499999999994</v>
       </c>
-      <c r="G9" s="34">
-        <f t="shared" si="1"/>
-        <v>0.27000000000001023</v>
-      </c>
+      <c r="G9" s="28"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -26396,29 +26544,26 @@
       <c r="Z9" s="9"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="21">
         <v>71.7</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="21">
         <v>72.37</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="21">
         <v>72.459999999999994</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="21">
         <v>72.569999999999993</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>72.274999999999991</v>
       </c>
-      <c r="G10" s="34">
-        <f t="shared" si="1"/>
-        <v>0.10999999999999943</v>
-      </c>
+      <c r="G10" s="28"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -26440,29 +26585,26 @@
       <c r="Z10" s="9"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="21">
         <v>71.25</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="21">
         <v>72.14</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="21">
         <v>72.33</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="21">
         <v>72.459999999999994</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>72.044999999999987</v>
       </c>
-      <c r="G11" s="34">
-        <f t="shared" si="1"/>
-        <v>0.12999999999999545</v>
-      </c>
+      <c r="G11" s="28"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -26484,29 +26626,26 @@
       <c r="Z11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="21">
         <v>70.86</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="21">
         <v>71.52</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="21">
         <v>71.510000000000005</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="21">
         <v>71.760000000000005</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
         <v>71.412499999999994</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
+      <c r="G12" s="28"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -26543,14 +26682,11 @@
       <c r="E13" s="11">
         <v>70.760000000000005</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>70.417500000000004</v>
       </c>
-      <c r="G13" s="34">
-        <f t="shared" si="1"/>
-        <v>0.15000000000000568</v>
-      </c>
+      <c r="G13" s="28"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -26587,14 +26723,11 @@
       <c r="E14" s="11">
         <v>70.03</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
         <v>69.852500000000006</v>
       </c>
-      <c r="G14" s="34">
-        <f t="shared" si="1"/>
-        <v>0.12999999999999545</v>
-      </c>
+      <c r="G14" s="28"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -26631,14 +26764,11 @@
       <c r="E15" s="11">
         <v>69.680000000000007</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="16">
         <f t="shared" si="0"/>
         <v>69.497500000000002</v>
       </c>
-      <c r="G15" s="34">
-        <f t="shared" si="1"/>
-        <v>0.21000000000000796</v>
-      </c>
+      <c r="G15" s="28"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -26660,29 +26790,26 @@
       <c r="Z15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="21">
         <v>68.599999999999994</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="21">
         <v>69.08</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="21">
         <v>69.08</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="21">
         <v>69.239999999999995</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="16">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="G16" s="34">
-        <f t="shared" si="1"/>
-        <v>0.15999999999999659</v>
-      </c>
+      <c r="G16" s="28"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -26719,14 +26846,11 @@
       <c r="E17" s="11">
         <v>69.23</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="16">
         <f t="shared" si="0"/>
         <v>68.915000000000006</v>
       </c>
-      <c r="G17" s="34">
-        <f t="shared" si="1"/>
-        <v>0.18999999999999773</v>
-      </c>
+      <c r="G17" s="28"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -26763,14 +26887,11 @@
       <c r="E18" s="11">
         <v>68.760000000000005</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="16">
         <f t="shared" si="0"/>
         <v>68.222499999999997</v>
       </c>
-      <c r="G18" s="34">
-        <f t="shared" si="1"/>
-        <v>0.27000000000001023</v>
-      </c>
+      <c r="G18" s="28"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -26807,14 +26928,11 @@
       <c r="E19" s="11">
         <v>67.86</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="16">
         <f t="shared" si="0"/>
         <v>67.557500000000005</v>
       </c>
-      <c r="G19" s="34">
-        <f t="shared" si="1"/>
-        <v>0.12000000000000455</v>
-      </c>
+      <c r="G19" s="28"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -26836,29 +26954,26 @@
       <c r="Z19" s="9"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="21">
         <v>65.599999999999994</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="21">
         <v>66.459999999999994</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="21">
         <v>66.64</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="21">
         <v>66.77</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="16">
         <f t="shared" si="0"/>
         <v>66.367499999999993</v>
       </c>
-      <c r="G20" s="34">
-        <f t="shared" si="1"/>
-        <v>0.12999999999999545</v>
-      </c>
+      <c r="G20" s="28"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -26880,29 +26995,26 @@
       <c r="Z20" s="9"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="21">
         <v>60.28</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="21">
         <v>61.26</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="21">
         <v>61.09</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="21">
         <v>61.35</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="16">
         <f t="shared" si="0"/>
         <v>60.994999999999997</v>
       </c>
-      <c r="G21" s="34">
-        <f t="shared" si="1"/>
-        <v>0.25999999999999801</v>
-      </c>
+      <c r="G21" s="28"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -26924,7 +27036,7 @@
       <c r="Z21" s="9"/>
     </row>
     <row r="22" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="F22" s="33"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>

</xml_diff>